<commit_message>
Upper case Browser Names
</commit_message>
<xml_diff>
--- a/examples/BaangtDBFill.xlsx
+++ b/examples/BaangtDBFill.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10209"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10308"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bernhardbuhl/git/baangt/examples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F363D91F-0A01-374A-A151-6CE9001149BB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FF10023-5A3C-A743-AA14-E784834A85C8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13460" yWindow="1160" windowWidth="18840" windowHeight="17760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-22120" yWindow="1760" windowWidth="18840" windowHeight="17760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TestStepExecution" sheetId="1" r:id="rId1"/>
@@ -81,9 +81,6 @@
     <t>Name</t>
   </si>
   <si>
-    <t>//a[contains(.,'+ new Test Step')]</t>
-  </si>
-  <si>
     <t>//input[contains(@name,'name')]</t>
   </si>
   <si>
@@ -241,6 +238,9 @@
   </si>
   <si>
     <t>//*[@id="description"]</t>
+  </si>
+  <si>
+    <t>//a[contains(.,'+ create Test Step')]</t>
   </si>
 </sst>
 </file>
@@ -640,7 +640,7 @@
   <dimension ref="A1:I15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -688,42 +688,42 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C3" t="s">
         <v>12</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" t="s">
+        <v>40</v>
+      </c>
+      <c r="F3" t="s">
         <v>41</v>
       </c>
-      <c r="F3" t="s">
-        <v>42</v>
-      </c>
       <c r="G3">
         <v>1</v>
       </c>
       <c r="H3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D5">
         <v>12345</v>
@@ -734,12 +734,12 @@
         <v>10</v>
       </c>
       <c r="C6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D7" s="1"/>
     </row>
@@ -756,29 +756,29 @@
         <v>10</v>
       </c>
       <c r="C9" t="s">
-        <v>16</v>
+        <v>69</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D10" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C11" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D11" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
@@ -786,7 +786,7 @@
         <v>10</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
@@ -794,15 +794,15 @@
         <v>10</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C14" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D14">
         <v>1</v>
@@ -813,7 +813,7 @@
         <v>10</v>
       </c>
       <c r="C15" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -846,19 +846,19 @@
         <v>15</v>
       </c>
       <c r="C1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D1" t="s">
         <v>18</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>19</v>
       </c>
-      <c r="E1" t="s">
-        <v>20</v>
-      </c>
       <c r="F1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
@@ -873,13 +873,13 @@
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E2" t="s">
         <v>15</v>
       </c>
       <c r="F2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G2" t="str">
         <f>B2&amp;" " &amp;E2 &amp; " " &amp;F2</f>
@@ -898,13 +898,13 @@
         <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G3" t="str">
         <f t="shared" ref="G3:G55" si="1">B3&amp;" " &amp;E3 &amp; " " &amp;F3</f>
@@ -923,13 +923,13 @@
         <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G4" t="str">
         <f t="shared" si="1"/>
@@ -948,13 +948,13 @@
         <v>1</v>
       </c>
       <c r="D5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G5" t="str">
         <f t="shared" si="1"/>
@@ -973,13 +973,13 @@
         <v>1</v>
       </c>
       <c r="D6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G6" t="str">
         <f t="shared" si="1"/>
@@ -998,13 +998,13 @@
         <v>1</v>
       </c>
       <c r="D7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G7" t="str">
         <f t="shared" si="1"/>
@@ -1023,13 +1023,13 @@
         <v>1</v>
       </c>
       <c r="D8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G8" t="str">
         <f t="shared" si="1"/>
@@ -1048,13 +1048,13 @@
         <v>1</v>
       </c>
       <c r="D9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G9" t="str">
         <f t="shared" si="1"/>
@@ -1073,13 +1073,13 @@
         <v>1</v>
       </c>
       <c r="D10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E10" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F10" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G10" t="str">
         <f t="shared" si="1"/>
@@ -1098,13 +1098,13 @@
         <v>1</v>
       </c>
       <c r="D11" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E11" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F11" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G11" t="str">
         <f t="shared" si="1"/>
@@ -1123,13 +1123,13 @@
         <v>1</v>
       </c>
       <c r="D12" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E12" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F12" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G12" t="str">
         <f t="shared" si="1"/>
@@ -1148,13 +1148,13 @@
         <v>1</v>
       </c>
       <c r="D13" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E13" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F13" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G13" t="str">
         <f t="shared" si="1"/>
@@ -1173,13 +1173,13 @@
         <v>1</v>
       </c>
       <c r="D14" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E14" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F14" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G14" t="str">
         <f t="shared" si="1"/>
@@ -1198,13 +1198,13 @@
         <v>1</v>
       </c>
       <c r="D15" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E15" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F15" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G15" t="str">
         <f t="shared" si="1"/>
@@ -1223,13 +1223,13 @@
         <v>1</v>
       </c>
       <c r="D16" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E16" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F16" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G16" t="str">
         <f t="shared" si="1"/>
@@ -1248,13 +1248,13 @@
         <v>1</v>
       </c>
       <c r="D17" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E17" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F17" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G17" t="str">
         <f t="shared" si="1"/>
@@ -1273,13 +1273,13 @@
         <v>1</v>
       </c>
       <c r="D18" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E18" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F18" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G18" t="str">
         <f t="shared" si="1"/>
@@ -1298,13 +1298,13 @@
         <v>1</v>
       </c>
       <c r="D19" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E19" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F19" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G19" t="str">
         <f t="shared" si="1"/>
@@ -1323,13 +1323,13 @@
         <v>1</v>
       </c>
       <c r="D20" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E20" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F20" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G20" t="str">
         <f t="shared" si="1"/>
@@ -1348,13 +1348,13 @@
         <v>1</v>
       </c>
       <c r="D21" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E21" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F21" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G21" t="str">
         <f t="shared" si="1"/>
@@ -1373,13 +1373,13 @@
         <v>1</v>
       </c>
       <c r="D22" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E22" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F22" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G22" t="str">
         <f t="shared" si="1"/>
@@ -1398,13 +1398,13 @@
         <v>1</v>
       </c>
       <c r="D23" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E23" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F23" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G23" t="str">
         <f t="shared" si="1"/>
@@ -1423,13 +1423,13 @@
         <v>1</v>
       </c>
       <c r="D24" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E24" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F24" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G24" t="str">
         <f t="shared" si="1"/>
@@ -1448,13 +1448,13 @@
         <v>1</v>
       </c>
       <c r="D25" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E25" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F25" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G25" t="str">
         <f t="shared" si="1"/>
@@ -1473,13 +1473,13 @@
         <v>1</v>
       </c>
       <c r="D26" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E26" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F26" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G26" t="str">
         <f t="shared" si="1"/>
@@ -1498,13 +1498,13 @@
         <v>1</v>
       </c>
       <c r="D27" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E27" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F27" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G27" t="str">
         <f t="shared" si="1"/>
@@ -1523,13 +1523,13 @@
         <v>1</v>
       </c>
       <c r="D28" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E28" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F28" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G28" t="str">
         <f t="shared" si="1"/>
@@ -1548,13 +1548,13 @@
         <v>1</v>
       </c>
       <c r="D29" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E29" t="s">
         <v>15</v>
       </c>
       <c r="F29" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G29" t="str">
         <f t="shared" si="1"/>
@@ -1573,13 +1573,13 @@
         <v>1</v>
       </c>
       <c r="D30" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E30" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F30" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G30" t="str">
         <f t="shared" si="1"/>
@@ -1598,13 +1598,13 @@
         <v>1</v>
       </c>
       <c r="D31" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E31" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F31" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G31" t="str">
         <f t="shared" si="1"/>
@@ -1623,13 +1623,13 @@
         <v>1</v>
       </c>
       <c r="D32" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E32" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F32" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G32" t="str">
         <f t="shared" si="1"/>
@@ -1648,13 +1648,13 @@
         <v>1</v>
       </c>
       <c r="D33" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E33" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F33" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G33" t="str">
         <f t="shared" si="1"/>
@@ -1673,13 +1673,13 @@
         <v>1</v>
       </c>
       <c r="D34" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E34" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F34" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G34" t="str">
         <f t="shared" si="1"/>
@@ -1698,13 +1698,13 @@
         <v>1</v>
       </c>
       <c r="D35" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E35" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F35" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G35" t="str">
         <f t="shared" si="1"/>
@@ -1723,13 +1723,13 @@
         <v>1</v>
       </c>
       <c r="D36" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E36" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F36" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G36" t="str">
         <f t="shared" si="1"/>
@@ -1748,13 +1748,13 @@
         <v>1</v>
       </c>
       <c r="D37" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E37" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F37" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G37" t="str">
         <f t="shared" si="1"/>
@@ -1773,13 +1773,13 @@
         <v>1</v>
       </c>
       <c r="D38" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E38" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F38" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G38" t="str">
         <f t="shared" si="1"/>
@@ -1798,13 +1798,13 @@
         <v>1</v>
       </c>
       <c r="D39" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E39" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F39" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G39" t="str">
         <f t="shared" si="1"/>
@@ -1823,13 +1823,13 @@
         <v>1</v>
       </c>
       <c r="D40" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E40" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F40" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G40" t="str">
         <f t="shared" si="1"/>
@@ -1848,13 +1848,13 @@
         <v>1</v>
       </c>
       <c r="D41" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E41" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F41" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G41" t="str">
         <f t="shared" si="1"/>
@@ -1873,13 +1873,13 @@
         <v>1</v>
       </c>
       <c r="D42" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E42" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F42" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G42" t="str">
         <f t="shared" si="1"/>
@@ -1898,13 +1898,13 @@
         <v>1</v>
       </c>
       <c r="D43" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E43" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F43" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G43" t="str">
         <f t="shared" si="1"/>
@@ -1923,13 +1923,13 @@
         <v>1</v>
       </c>
       <c r="D44" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E44" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F44" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G44" t="str">
         <f t="shared" si="1"/>
@@ -1948,13 +1948,13 @@
         <v>1</v>
       </c>
       <c r="D45" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E45" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F45" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G45" t="str">
         <f t="shared" si="1"/>
@@ -1973,13 +1973,13 @@
         <v>1</v>
       </c>
       <c r="D46" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E46" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F46" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G46" t="str">
         <f t="shared" si="1"/>
@@ -1998,13 +1998,13 @@
         <v>1</v>
       </c>
       <c r="D47" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E47" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F47" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G47" t="str">
         <f t="shared" si="1"/>
@@ -2023,13 +2023,13 @@
         <v>1</v>
       </c>
       <c r="D48" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E48" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F48" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G48" t="str">
         <f t="shared" si="1"/>
@@ -2048,13 +2048,13 @@
         <v>1</v>
       </c>
       <c r="D49" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E49" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F49" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G49" t="str">
         <f t="shared" si="1"/>
@@ -2073,13 +2073,13 @@
         <v>1</v>
       </c>
       <c r="D50" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E50" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F50" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G50" t="str">
         <f t="shared" si="1"/>
@@ -2098,13 +2098,13 @@
         <v>1</v>
       </c>
       <c r="D51" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E51" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F51" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G51" t="str">
         <f t="shared" si="1"/>
@@ -2123,13 +2123,13 @@
         <v>1</v>
       </c>
       <c r="D52" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E52" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F52" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G52" t="str">
         <f t="shared" si="1"/>
@@ -2148,13 +2148,13 @@
         <v>1</v>
       </c>
       <c r="D53" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E53" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F53" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G53" t="str">
         <f t="shared" si="1"/>
@@ -2173,13 +2173,13 @@
         <v>1</v>
       </c>
       <c r="D54" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E54" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F54" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G54" t="str">
         <f t="shared" si="1"/>
@@ -2198,13 +2198,13 @@
         <v>1</v>
       </c>
       <c r="D55" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E55" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F55" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G55" t="str">
         <f t="shared" si="1"/>

</xml_diff>